<commit_message>
add date calendar in excel
</commit_message>
<xml_diff>
--- a/3MLAHP.xlsx
+++ b/3MLAHP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ollama-project\3MLAHP\3MLAHP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DCD11C-2EE7-4FFE-A7A0-9BA9FB8D49D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC5FF3D-450A-4D87-B82F-31D70BCFEDF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{7BDC706B-0A83-48A8-B4D0-F706747B6421}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7BDC706B-0A83-48A8-B4D0-F706747B6421}"/>
   </bookViews>
   <sheets>
     <sheet name="Booking" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Chopper_Plan" sheetId="3" r:id="rId3"/>
     <sheet name="Field_Bed_Capacity" sheetId="4" r:id="rId4"/>
     <sheet name="Regular_Crew" sheetId="6" r:id="rId5"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId6"/>
+    <sheet name="Date_Calendar" sheetId="7" r:id="rId6"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId7"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6461" uniqueCount="1219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6463" uniqueCount="1221">
   <si>
     <t>Field</t>
   </si>
@@ -3707,14 +3707,21 @@
   </si>
   <si>
     <t>Person_On_Board</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="\⏩\ @"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -3771,7 +3778,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3805,11 +3812,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="14">
+    <dxf>
+      <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -4028,7 +4042,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7DEF7D4C-5B74-4D4B-A123-18AF15B47356}" name="VesselChopperPlan" displayName="VesselChopperPlan" ref="A1:O125" totalsRowShown="0" headerRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7DEF7D4C-5B74-4D4B-A123-18AF15B47356}" name="VesselChopperPlan" displayName="VesselChopperPlan" ref="A1:O125" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A1:O125" xr:uid="{7DEF7D4C-5B74-4D4B-A123-18AF15B47356}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O104">
     <sortCondition ref="F1:F125"/>
@@ -4037,20 +4051,31 @@
     <tableColumn id="1" xr3:uid="{E4BF458C-27B3-4CD1-B40B-DF6C29EE9275}" name="Type"/>
     <tableColumn id="3" xr3:uid="{0EDD59AF-2CA4-4CED-9962-C2C4F0EC0EE8}" name="Boat_Name"/>
     <tableColumn id="4" xr3:uid="{18CBA53F-9240-4C52-8765-179A46AF12A4}" name="Direction"/>
-    <tableColumn id="5" xr3:uid="{703414AF-D622-46DC-900F-68A2C47B42F6}" name="Origin" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{8835E596-0EC6-4B5A-B5D6-F9E639FF2FA1}" name="Destination" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{3F960198-6C70-4153-A514-B72467E91E9D}" name="DEP._x000a_Date" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{9970134C-AA2D-4545-9167-34A72CCB7BC0}" name="DEP._x000a_Time" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{D21BEB48-14F6-4155-AD5F-E6B3EC447ED3}" name="ARR_x000a_Date" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{553535AA-681E-4884-B3F1-E45480AF0196}" name="ARR_x000a_Time" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{80EAA342-D668-46EA-9412-D79586BBA746}" name="MAX SEAT" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{E014387B-BD05-46BA-A0F9-91E3A21C6DAA}" name="Regular Crew" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{D1C17298-F355-495B-BCD0-0303F1161A5D}" name="BOOK SEAT" dataDxfId="3"/>
-    <tableColumn id="14" xr3:uid="{BFFBC9D9-7C3A-44DE-9A12-ECD0B0CF5F59}" name="AVAILABLE SEAT" dataDxfId="2"/>
-    <tableColumn id="22" xr3:uid="{B6C648EA-CDFE-491E-AEE2-50B3FDFE9B0F}" name="Code" dataDxfId="1"/>
-    <tableColumn id="21" xr3:uid="{A10F0A84-BADD-46D8-8A9D-59E4108BA134}" name="Trip ID" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{703414AF-D622-46DC-900F-68A2C47B42F6}" name="Origin" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{8835E596-0EC6-4B5A-B5D6-F9E639FF2FA1}" name="Destination" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{3F960198-6C70-4153-A514-B72467E91E9D}" name="DEP._x000a_Date" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{9970134C-AA2D-4545-9167-34A72CCB7BC0}" name="DEP._x000a_Time" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{D21BEB48-14F6-4155-AD5F-E6B3EC447ED3}" name="ARR_x000a_Date" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{553535AA-681E-4884-B3F1-E45480AF0196}" name="ARR_x000a_Time" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{80EAA342-D668-46EA-9412-D79586BBA746}" name="MAX SEAT" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{E014387B-BD05-46BA-A0F9-91E3A21C6DAA}" name="Regular Crew" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{D1C17298-F355-495B-BCD0-0303F1161A5D}" name="BOOK SEAT" dataDxfId="4"/>
+    <tableColumn id="14" xr3:uid="{BFFBC9D9-7C3A-44DE-9A12-ECD0B0CF5F59}" name="AVAILABLE SEAT" dataDxfId="3"/>
+    <tableColumn id="22" xr3:uid="{B6C648EA-CDFE-491E-AEE2-50B3FDFE9B0F}" name="Code" dataDxfId="2"/>
+    <tableColumn id="21" xr3:uid="{A10F0A84-BADD-46D8-8A9D-59E4108BA134}" name="Trip ID" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A0A5921B-75C6-4D50-A625-0DA889163F1B}" name="Date_Calendar" displayName="Date_Calendar" ref="A1:B93" totalsRowShown="0">
+  <autoFilter ref="A1:B93" xr:uid="{71BBF952-CB0E-49B3-8380-0B0F6974CD7E}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{774682A5-3F96-41D2-B3C4-67E810EA6EEA}" name="Id"/>
+    <tableColumn id="2" xr3:uid="{61972759-FBFD-430B-8C94-09F4F402A67E}" name="Date" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -4353,8 +4378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{510B1057-B73F-4731-AE0F-D1F8C5623A92}">
   <dimension ref="A1:R167"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39558,7 +39583,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5977777-19BE-4DC8-AB02-3481AA575734}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
@@ -40223,13 +40248,1046 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56805C11-6231-475D-B94F-A391C500FD99}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF830692-B569-4322-AC16-980EF9D6880B}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:G186"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E99" sqref="E99"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13">
+        <v>45839</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="13">
+        <v>45840</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13">
+        <v>45841</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="13">
+        <v>45842</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="13">
+        <v>45843</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="13">
+        <v>45844</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="13">
+        <v>45845</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="13">
+        <v>45846</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="13">
+        <v>45847</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="13">
+        <v>45848</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="13">
+        <v>45849</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="13">
+        <v>45850</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="13">
+        <v>45851</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="13">
+        <v>45852</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="13">
+        <v>45853</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="13">
+        <v>45854</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="13">
+        <v>45855</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="13">
+        <v>45856</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="13">
+        <v>45857</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="13">
+        <v>45858</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="13">
+        <v>45859</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="13">
+        <v>45860</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="13">
+        <v>45861</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="13">
+        <v>45862</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="13">
+        <v>45863</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="13">
+        <v>45864</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="13">
+        <v>45865</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="13">
+        <v>45866</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="13">
+        <v>45867</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="13">
+        <v>45868</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="13">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="13">
+        <v>45870</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="13">
+        <v>45871</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="13">
+        <v>45872</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="13">
+        <v>45873</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="13">
+        <v>45874</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" s="13">
+        <v>45875</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" s="13">
+        <v>45876</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" s="13">
+        <v>45877</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" s="13">
+        <v>45878</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" s="13">
+        <v>45879</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" s="13">
+        <v>45880</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" s="13">
+        <v>45881</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" s="13">
+        <v>45882</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" s="13">
+        <v>45883</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" s="13">
+        <v>45884</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" s="13">
+        <v>45885</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" s="13">
+        <v>45886</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" s="13">
+        <v>45887</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" s="13">
+        <v>45888</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" s="13">
+        <v>45889</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" s="13">
+        <v>45890</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" s="13">
+        <v>45891</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" s="13">
+        <v>45892</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" s="13">
+        <v>45893</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" s="13">
+        <v>45894</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" s="13">
+        <v>45895</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" s="13">
+        <v>45896</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" s="13">
+        <v>45897</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" s="13">
+        <v>45898</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" s="13">
+        <v>45899</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" s="13">
+        <v>45900</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" s="13">
+        <v>45901</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" s="13">
+        <v>45902</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" s="13">
+        <v>45903</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" s="13">
+        <v>45904</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" s="13">
+        <v>45905</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" s="13">
+        <v>45906</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" s="13">
+        <v>45907</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" s="13">
+        <v>45908</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" s="13">
+        <v>45909</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" s="13">
+        <v>45910</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" s="13">
+        <v>45911</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" s="13">
+        <v>45912</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" s="13">
+        <v>45913</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" s="13">
+        <v>45914</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" s="13">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" s="13">
+        <v>45916</v>
+      </c>
+      <c r="G79" s="14"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" s="13">
+        <v>45917</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" s="13">
+        <v>45918</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" s="13">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" s="13">
+        <v>45920</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" s="13">
+        <v>45921</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" s="13">
+        <v>45922</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" s="13">
+        <v>45923</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" s="13">
+        <v>45924</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" s="13">
+        <v>45925</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" s="13">
+        <v>45926</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" s="13">
+        <v>45927</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" s="13">
+        <v>45928</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" s="13">
+        <v>45929</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" s="13">
+        <v>45930</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C96" s="1"/>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C97" s="1"/>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C98" s="1"/>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C99" s="1"/>
+    </row>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C100" s="1"/>
+    </row>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C101" s="1"/>
+    </row>
+    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C102" s="1"/>
+    </row>
+    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C103" s="1"/>
+    </row>
+    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C104" s="1"/>
+    </row>
+    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C105" s="1"/>
+    </row>
+    <row r="106" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C106" s="1"/>
+    </row>
+    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C107" s="1"/>
+    </row>
+    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C108" s="1"/>
+    </row>
+    <row r="109" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C109" s="1"/>
+    </row>
+    <row r="110" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C110" s="1"/>
+    </row>
+    <row r="111" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C111" s="1"/>
+    </row>
+    <row r="112" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C112" s="1"/>
+    </row>
+    <row r="113" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C113" s="1"/>
+    </row>
+    <row r="114" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C114" s="1"/>
+    </row>
+    <row r="115" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C115" s="1"/>
+    </row>
+    <row r="116" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C116" s="1"/>
+    </row>
+    <row r="117" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C117" s="1"/>
+    </row>
+    <row r="118" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C118" s="1"/>
+    </row>
+    <row r="119" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C119" s="1"/>
+    </row>
+    <row r="120" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C120" s="1"/>
+    </row>
+    <row r="121" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C121" s="1"/>
+    </row>
+    <row r="122" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C122" s="1"/>
+    </row>
+    <row r="123" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C123" s="1"/>
+    </row>
+    <row r="124" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C124" s="1"/>
+    </row>
+    <row r="125" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C125" s="1"/>
+    </row>
+    <row r="126" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C126" s="1"/>
+    </row>
+    <row r="127" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C127" s="1"/>
+    </row>
+    <row r="128" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C128" s="1"/>
+    </row>
+    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C129" s="1"/>
+    </row>
+    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C130" s="1"/>
+    </row>
+    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C131" s="1"/>
+    </row>
+    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C132" s="1"/>
+    </row>
+    <row r="133" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C133" s="1"/>
+    </row>
+    <row r="134" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C134" s="1"/>
+    </row>
+    <row r="135" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C135" s="1"/>
+    </row>
+    <row r="136" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C136" s="1"/>
+    </row>
+    <row r="137" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C137" s="1"/>
+    </row>
+    <row r="138" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C138" s="1"/>
+    </row>
+    <row r="139" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C139" s="1"/>
+    </row>
+    <row r="140" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C140" s="1"/>
+    </row>
+    <row r="141" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C141" s="1"/>
+    </row>
+    <row r="142" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C142" s="1"/>
+    </row>
+    <row r="143" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C143" s="1"/>
+    </row>
+    <row r="144" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C144" s="1"/>
+    </row>
+    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C145" s="1"/>
+    </row>
+    <row r="146" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C146" s="1"/>
+    </row>
+    <row r="147" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C147" s="1"/>
+    </row>
+    <row r="148" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C148" s="1"/>
+    </row>
+    <row r="149" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C149" s="1"/>
+    </row>
+    <row r="150" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C150" s="1"/>
+    </row>
+    <row r="151" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C151" s="1"/>
+    </row>
+    <row r="152" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C152" s="1"/>
+    </row>
+    <row r="153" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C153" s="1"/>
+    </row>
+    <row r="154" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C154" s="1"/>
+    </row>
+    <row r="155" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C155" s="1"/>
+    </row>
+    <row r="156" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C156" s="1"/>
+    </row>
+    <row r="157" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C157" s="1"/>
+    </row>
+    <row r="158" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C158" s="1"/>
+    </row>
+    <row r="159" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C159" s="1"/>
+    </row>
+    <row r="160" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C160" s="1"/>
+    </row>
+    <row r="161" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C161" s="1"/>
+    </row>
+    <row r="162" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C162" s="1"/>
+    </row>
+    <row r="163" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C163" s="1"/>
+    </row>
+    <row r="164" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C164" s="1"/>
+    </row>
+    <row r="165" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C165" s="1"/>
+    </row>
+    <row r="166" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C166" s="1"/>
+    </row>
+    <row r="167" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C167" s="1"/>
+    </row>
+    <row r="168" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C168" s="1"/>
+    </row>
+    <row r="169" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C169" s="1"/>
+    </row>
+    <row r="170" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C170" s="1"/>
+    </row>
+    <row r="171" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C171" s="1"/>
+    </row>
+    <row r="172" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C172" s="1"/>
+    </row>
+    <row r="173" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C173" s="1"/>
+    </row>
+    <row r="174" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C174" s="1"/>
+    </row>
+    <row r="175" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C175" s="1"/>
+    </row>
+    <row r="176" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C176" s="1"/>
+    </row>
+    <row r="177" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C177" s="1"/>
+    </row>
+    <row r="178" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C178" s="1"/>
+    </row>
+    <row r="179" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C179" s="1"/>
+    </row>
+    <row r="180" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C180" s="1"/>
+    </row>
+    <row r="181" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C181" s="1"/>
+    </row>
+    <row r="182" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C182" s="1"/>
+    </row>
+    <row r="183" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C183" s="1"/>
+    </row>
+    <row r="184" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C184" s="1"/>
+    </row>
+    <row r="185" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C185" s="1"/>
+    </row>
+    <row r="186" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C186" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>